<commit_message>
Initial push of OCR app with domain/service/ui structure
</commit_message>
<xml_diff>
--- a/template_output.xlsx
+++ b/template_output.xlsx
@@ -1270,7 +1270,11 @@
           <t>法人名</t>
         </is>
       </c>
-      <c r="B1" s="71" t="n"/>
+      <c r="B1" s="71" t="inlineStr">
+        <is>
+          <t>渡辺株式会社</t>
+        </is>
+      </c>
       <c r="C1" s="86" t="n"/>
       <c r="D1" s="87" t="n"/>
     </row>
@@ -1574,11 +1578,31 @@
           <t>一律</t>
         </is>
       </c>
-      <c r="B21" s="44" t="n"/>
-      <c r="C21" s="50" t="n"/>
-      <c r="D21" s="44" t="n"/>
-      <c r="E21" s="44" t="n"/>
-      <c r="F21" s="44" t="n"/>
+      <c r="B21" s="44" t="inlineStr">
+        <is>
+          <t>53462</t>
+        </is>
+      </c>
+      <c r="C21" s="50" t="inlineStr">
+        <is>
+          <t>58907</t>
+        </is>
+      </c>
+      <c r="D21" s="44" t="inlineStr">
+        <is>
+          <t>60872</t>
+        </is>
+      </c>
+      <c r="E21" s="44" t="inlineStr">
+        <is>
+          <t>29383</t>
+        </is>
+      </c>
+      <c r="F21" s="44" t="inlineStr">
+        <is>
+          <t>28637</t>
+        </is>
+      </c>
       <c r="G21" s="44" t="n"/>
       <c r="H21" s="44" t="n"/>
       <c r="I21" s="44" t="n"/>

</xml_diff>

<commit_message>
set python version for render
</commit_message>
<xml_diff>
--- a/template_output.xlsx
+++ b/template_output.xlsx
@@ -1579,26 +1579,10 @@
           <t>53462</t>
         </is>
       </c>
-      <c r="C21" s="50" t="inlineStr">
-        <is>
-          <t>58907</t>
-        </is>
-      </c>
-      <c r="D21" s="44" t="inlineStr">
-        <is>
-          <t>60872</t>
-        </is>
-      </c>
-      <c r="E21" s="44" t="inlineStr">
-        <is>
-          <t>29383</t>
-        </is>
-      </c>
-      <c r="F21" s="44" t="inlineStr">
-        <is>
-          <t>28637</t>
-        </is>
-      </c>
+      <c r="C21" s="50" t="inlineStr"/>
+      <c r="D21" s="44" t="inlineStr"/>
+      <c r="E21" s="44" t="inlineStr"/>
+      <c r="F21" s="44" t="inlineStr"/>
       <c r="G21" s="44" t="inlineStr"/>
       <c r="H21" s="44" t="inlineStr"/>
       <c r="I21" s="44" t="inlineStr"/>

</xml_diff>